<commit_message>
add data and plans
</commit_message>
<xml_diff>
--- a/days_map_plans.xlsx
+++ b/days_map_plans.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Franc\Documents\Projects\30_day_maps_challenge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D071854-DE4E-49C5-8BDC-AC8C356245AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91485115-4848-435C-85CF-3C3F492B4354}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9150" yWindow="1222" windowWidth="8618" windowHeight="13058" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
   <si>
     <t>Day</t>
   </si>
@@ -135,23 +136,94 @@
     <t>pedestrian &amp; biking injuries in San Antonio</t>
   </si>
   <si>
-    <t>macau map</t>
-  </si>
-  <si>
     <t>https://searchworks.stanford.edu/view/11754993</t>
+  </si>
+  <si>
+    <t>population as a choropleth in SA metro</t>
+  </si>
+  <si>
+    <t>Denver neighborhoods mental map</t>
+  </si>
+  <si>
+    <t>trip to Denver CO</t>
+  </si>
+  <si>
+    <t>https://www.andersondesigngroupstore.com/a/collections/American-State-Pride/texas-map-vintage/6308831002775</t>
+  </si>
+  <si>
+    <t>Africa population map</t>
+  </si>
+  <si>
+    <t>North America population map</t>
+  </si>
+  <si>
+    <t>South America population map</t>
+  </si>
+  <si>
+    <t>Asia population/urbanization map</t>
+  </si>
+  <si>
+    <t>https://twitter.com/JohnLeFevre/status/1707172630220919287/photo/1</t>
+  </si>
+  <si>
+    <t>https://twitter.com/rappa753/status/1701234203004649929/photo/2</t>
+  </si>
+  <si>
+    <t>Land use in a neighborhood</t>
+  </si>
+  <si>
+    <t>https://x.com/gmapsmania/status/1691123505289461760?s=20</t>
+  </si>
+  <si>
+    <t>heb vs walmart markets</t>
+  </si>
+  <si>
+    <t>bank density or top lifestyle segment per hexagon</t>
+  </si>
+  <si>
+    <t>classic state of texas map</t>
+  </si>
+  <si>
+    <t>European population map</t>
+  </si>
+  <si>
+    <t>Oceania urbanization map</t>
+  </si>
+  <si>
+    <t>Flows to TX Metro / Comal County</t>
+  </si>
+  <si>
+    <t>weather/climate</t>
+  </si>
+  <si>
+    <t>trails/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -174,8 +246,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -458,20 +538,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="3.796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.53125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.6640625" style="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
     </row>
@@ -482,18 +567,18 @@
       <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C2" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>35</v>
       </c>
     </row>
@@ -504,35 +589,47 @@
       <c r="B4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C5" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" t="s">
         <v>36</v>
       </c>
-      <c r="D6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="7" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.45">
@@ -542,6 +639,9 @@
       <c r="B8" t="s">
         <v>9</v>
       </c>
+      <c r="C8" s="1" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9">
@@ -550,21 +650,33 @@
       <c r="B9" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C9" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C10" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>12</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.45">
@@ -574,13 +686,22 @@
       <c r="B12" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C12" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
         <v>14</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.45">
@@ -598,6 +719,9 @@
       <c r="B15" t="s">
         <v>16</v>
       </c>
+      <c r="C15" s="1" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16">
@@ -607,31 +731,40 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C17" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C18" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="D19" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>19</v>
       </c>
@@ -639,15 +772,18 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="D21" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>21</v>
       </c>
@@ -655,7 +791,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>22</v>
       </c>
@@ -663,7 +799,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A24">
         <v>23</v>
       </c>
@@ -671,7 +807,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A25">
         <v>24</v>
       </c>
@@ -679,7 +815,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A26">
         <v>25</v>
       </c>
@@ -687,7 +823,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A27">
         <v>26</v>
       </c>
@@ -695,7 +831,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A28">
         <v>27</v>
       </c>
@@ -703,15 +839,18 @@
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="D29" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A30">
         <v>29</v>
       </c>
@@ -719,7 +858,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A31">
         <v>30</v>
       </c>
@@ -727,9 +866,27 @@
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A33" t="s">
+    <row r="33" spans="3:3" x14ac:dyDescent="0.45">
+      <c r="C33" t="s">
         <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7D7B62-E1FA-4E41-AEDB-CEE524CD049C}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:1" ht="57" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>